<commit_message>
Group 4 Data Dictionary
</commit_message>
<xml_diff>
--- a/Resources/Group4 Data Dictionary.xlsx
+++ b/Resources/Group4 Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6119fd54d26125e1/Desktop/BCamp Class Folder/GROUP 4 PROJECT/DATASETS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="222" documentId="8_{9E8DC3C9-BDE1-40AB-85CD-5646FD191401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74E80102-87F1-4731-BA8A-E691ACE65A99}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="8_{9E8DC3C9-BDE1-40AB-85CD-5646FD191401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15FDAE37-F1F7-4F68-8DB5-F7EC91539922}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{91026ABD-38E3-49E4-B77A-E5EC801C670E}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>STATE_AREA</t>
   </si>
   <si>
-    <t>STATE_NAME</t>
-  </si>
-  <si>
     <t>Measurement of state's land area by square miles.</t>
   </si>
   <si>
@@ -66,15 +63,6 @@
     <t>US States (not inclusive of US territories) - abbreviated.</t>
   </si>
   <si>
-    <t>Sex [Female; Male]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Race [American Indian/Alaska Native; Asian; Black; Native Hawaiian/Other Pacific Islander; White; Multiple/Other]. </t>
-  </si>
-  <si>
-    <t>Age group [0 - 17 years; 18 - 49 years; 50 - 64 years; 65 + years].</t>
-  </si>
-  <si>
     <t>POPULATION</t>
   </si>
   <si>
@@ -87,9 +75,6 @@
     <t>POLITICAL_PARTY</t>
   </si>
   <si>
-    <t>Potus Poll [Trump approval; Trump disapproval; Don't Care].</t>
-  </si>
-  <si>
     <t>POLITICAL_CREDO</t>
   </si>
   <si>
@@ -416,6 +401,121 @@
   </si>
   <si>
     <t>A median household income refers to the income level earned above or below half of the homes in the state giving a sense for a state's actual economic status.</t>
+  </si>
+  <si>
+    <r>
+      <t>Potus Poll [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1" tint="0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Trump approval; Trump disapproval; Don't Care</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1" tint="0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Sex [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1" tint="0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Female; Male; No ID</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1" tint="0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Age group [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1" tint="0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 - 17 years; 18 - 49 years; 50 - 64 years; 65 + years; No ID</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1" tint="0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Race [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1" tint="0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>American Indian/Alaska Native; Asian; Black; Native Hawaiian/Other Pacific Islander; White; Multiple/Other; No ID</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1" tint="0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">]. </t>
+    </r>
+  </si>
+  <si>
+    <t>ST</t>
   </si>
 </sst>
 </file>
@@ -857,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2FB1DDD-1FFB-4217-8B2F-863A3CC4485D}">
   <dimension ref="B1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,46 +973,46 @@
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -920,43 +1020,43 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -964,10 +1064,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -975,157 +1075,158 @@
         <v>3</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>